<commit_message>
Added trycatch blocks for xlsx implementation
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t xml:space="preserve">file</t>
   </si>
@@ -37,9 +37,15 @@
     <t xml:space="preserve">new</t>
   </si>
   <si>
+    <t xml:space="preserve">these comments</t>
+  </si>
+  <si>
     <t xml:space="preserve">blank</t>
   </si>
   <si>
+    <t xml:space="preserve">this is a blank</t>
+  </si>
+  <si>
     <t xml:space="preserve">test/test.r</t>
   </si>
   <si>
@@ -73,6 +79,9 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
+    <t xml:space="preserve">comenting</t>
+  </si>
+  <si>
     <t xml:space="preserve">write_csv(data.frame(dtst), here("test/dat/test.csv"))</t>
   </si>
   <si>
@@ -97,10 +106,26 @@
     <t xml:space="preserve">comments</t>
   </si>
   <si>
+    <t xml:space="preserve">comments 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">this is a coment</t>
   </si>
   <si>
     <t xml:space="preserve">this is a second comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is a
+multiline comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jkj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+this is a comment
+that is outside of the the code block
+</t>
   </si>
   <si>
     <t xml:space="preserve">this is a
@@ -556,10 +581,13 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -574,13 +602,18 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3"/>
-      <c r="C3"/>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
       <c r="D3" s="1" t="n">
         <v>44659</v>
       </c>
@@ -588,15 +621,18 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4"/>
-      <c r="C4"/>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
       <c r="D4" s="1" t="n">
         <v>44659</v>
       </c>
@@ -604,15 +640,18 @@
         <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5"/>
-      <c r="C5"/>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
       <c r="D5" s="1" t="n">
         <v>44659</v>
       </c>
@@ -620,8 +659,9 @@
         <v>0</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -639,7 +679,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -656,7 +696,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -671,9 +711,11 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3"/>
+        <v>13</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
       <c r="C3" s="1" t="n">
         <v>44659</v>
       </c>
@@ -681,14 +723,16 @@
         <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4"/>
+        <v>14</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
       <c r="C4" s="1" t="n">
         <v>44659</v>
       </c>
@@ -696,14 +740,16 @@
         <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5"/>
+        <v>15</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
       <c r="C5" s="1" t="n">
         <v>44659</v>
       </c>
@@ -711,14 +757,16 @@
         <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6"/>
+        <v>16</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
       <c r="C6" s="1" t="n">
         <v>44659</v>
       </c>
@@ -726,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -748,13 +796,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -768,19 +816,22 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -792,21 +843,24 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
+      <c r="I2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3"/>
+        <v>22</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
       <c r="F3" s="1" t="n">
         <v>44659</v>
       </c>
@@ -814,23 +868,26 @@
         <v>0</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4"/>
+        <v>22</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
       <c r="F4" s="1" t="n">
         <v>44659</v>
       </c>
@@ -838,23 +895,26 @@
         <v>0</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5"/>
+        <v>22</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
       <c r="F5" s="1" t="n">
         <v>44659</v>
       </c>
@@ -862,23 +922,26 @@
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6"/>
+        <v>26</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
       <c r="F6" s="1" t="n">
         <v>44659</v>
       </c>
@@ -886,23 +949,26 @@
         <v>0</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7"/>
+        <v>26</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
       <c r="F7" s="1" t="n">
         <v>44659</v>
       </c>
@@ -910,8 +976,9 @@
         <v>0</v>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -932,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -946,13 +1013,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -964,15 +1034,18 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
+      <c r="G2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3"/>
+        <v>30</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
       <c r="D3" s="1" t="n">
         <v>44659</v>
       </c>
@@ -980,17 +1053,20 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4"/>
+        <v>31</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
       <c r="D4" s="1" t="n">
         <v>44659</v>
       </c>
@@ -998,44 +1074,91 @@
         <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5"/>
+        <v>32</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
       <c r="D5" s="1" t="n">
         <v>44659</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6"/>
+        <v>34</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
       <c r="D6" s="1" t="n">
         <v>44659</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" s="1" t="n">
+        <v>44659</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" s="1" t="n">
+        <v>44659</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1056,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1073,10 +1196,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1091,12 +1214,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3"/>
+        <v>38</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
       <c r="D3" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1104,17 +1229,19 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4"/>
+        <v>38</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
       <c r="D4" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1122,7 +1249,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1141,25 +1268,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -1176,22 +1303,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -1209,16 +1336,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="n">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -1227,7 +1354,9 @@
       <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c r="H3"/>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
       <c r="I3" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1235,32 +1364,34 @@
         <v>0</v>
       </c>
       <c r="K3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="n">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
       </c>
-      <c r="H4"/>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
       <c r="I4" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1268,32 +1399,34 @@
         <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" t="n">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
       </c>
-      <c r="H5"/>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
       <c r="I5" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1301,32 +1434,34 @@
         <v>0</v>
       </c>
       <c r="K5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
       </c>
-      <c r="H6"/>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
       <c r="I6" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1334,32 +1469,34 @@
         <v>0</v>
       </c>
       <c r="K6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
-      <c r="H7"/>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
       <c r="I7" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1367,32 +1504,34 @@
         <v>0</v>
       </c>
       <c r="K7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
       </c>
-      <c r="H8"/>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
       <c r="I8" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1400,32 +1539,34 @@
         <v>0</v>
       </c>
       <c r="K8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
       </c>
-      <c r="H9"/>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
       <c r="I9" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1433,32 +1574,34 @@
         <v>0</v>
       </c>
       <c r="K9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" t="n">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
       </c>
-      <c r="H10"/>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
       <c r="I10" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1466,32 +1609,34 @@
         <v>0</v>
       </c>
       <c r="K10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11" t="n">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
       </c>
-      <c r="H11"/>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
       <c r="I11" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1499,32 +1644,34 @@
         <v>0</v>
       </c>
       <c r="K11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" t="n">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G12" t="n">
         <v>1</v>
       </c>
-      <c r="H12"/>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
       <c r="I12" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1532,32 +1679,34 @@
         <v>0</v>
       </c>
       <c r="K12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="n">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
       </c>
-      <c r="H13"/>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
       <c r="I13" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1565,32 +1714,34 @@
         <v>0</v>
       </c>
       <c r="K13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="n">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
       </c>
-      <c r="H14"/>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
       <c r="I14" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1598,21 +1749,21 @@
         <v>0</v>
       </c>
       <c r="K14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="n">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E15" t="n">
         <v>2</v>
@@ -1621,7 +1772,9 @@
       <c r="G15" t="n">
         <v>2</v>
       </c>
-      <c r="H15"/>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
       <c r="I15" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1629,32 +1782,34 @@
         <v>0</v>
       </c>
       <c r="K15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E16" t="n">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
       </c>
-      <c r="H16"/>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
       <c r="I16" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1662,32 +1817,34 @@
         <v>0</v>
       </c>
       <c r="K16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" t="n">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E17" t="n">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G17" t="n">
         <v>1</v>
       </c>
-      <c r="H17"/>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
       <c r="I17" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1695,32 +1852,34 @@
         <v>0</v>
       </c>
       <c r="K17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B18" t="n">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E18" t="n">
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
       </c>
-      <c r="H18"/>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
       <c r="I18" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1728,32 +1887,34 @@
         <v>0</v>
       </c>
       <c r="K18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B19" t="n">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E19" t="n">
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
       </c>
-      <c r="H19"/>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
       <c r="I19" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1761,32 +1922,34 @@
         <v>0</v>
       </c>
       <c r="K19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" t="n">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E20" t="n">
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
       </c>
-      <c r="H20"/>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
       <c r="I20" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1794,21 +1957,21 @@
         <v>0</v>
       </c>
       <c r="K20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B21" t="n">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E21" t="n">
         <v>2</v>
@@ -1817,7 +1980,9 @@
       <c r="G21" t="n">
         <v>2</v>
       </c>
-      <c r="H21"/>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
       <c r="I21" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1825,32 +1990,34 @@
         <v>0</v>
       </c>
       <c r="K21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B22" t="n">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E22" t="n">
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G22" t="n">
         <v>1</v>
       </c>
-      <c r="H22"/>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
       <c r="I22" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1858,32 +2025,34 @@
         <v>0</v>
       </c>
       <c r="K22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B23" t="n">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E23" t="n">
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
       </c>
-      <c r="H23"/>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
       <c r="I23" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1891,32 +2060,34 @@
         <v>0</v>
       </c>
       <c r="K23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B24" t="n">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G24" t="n">
         <v>1</v>
       </c>
-      <c r="H24"/>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
       <c r="I24" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1924,32 +2095,34 @@
         <v>0</v>
       </c>
       <c r="K24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B25" t="n">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E25" t="n">
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G25" t="n">
         <v>1</v>
       </c>
-      <c r="H25"/>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
       <c r="I25" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1957,32 +2130,34 @@
         <v>0</v>
       </c>
       <c r="K25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B26" t="n">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E26" t="n">
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G26" t="n">
         <v>1</v>
       </c>
-      <c r="H26"/>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
       <c r="I26" s="1" t="n">
         <v>44659</v>
       </c>
@@ -1990,32 +2165,34 @@
         <v>0</v>
       </c>
       <c r="K26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B27" t="n">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G27" t="n">
         <v>1</v>
       </c>
-      <c r="H27"/>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
       <c r="I27" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2023,32 +2200,34 @@
         <v>0</v>
       </c>
       <c r="K27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B28" t="n">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G28" t="n">
         <v>1</v>
       </c>
-      <c r="H28"/>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
       <c r="I28" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2056,32 +2235,34 @@
         <v>0</v>
       </c>
       <c r="K28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B29" t="n">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G29" t="n">
         <v>1</v>
       </c>
-      <c r="H29"/>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
       <c r="I29" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2089,32 +2270,34 @@
         <v>0</v>
       </c>
       <c r="K29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B30" t="n">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G30" t="n">
         <v>1</v>
       </c>
-      <c r="H30"/>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
       <c r="I30" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2122,32 +2305,34 @@
         <v>0</v>
       </c>
       <c r="K30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B31" t="n">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
       </c>
-      <c r="H31"/>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
       <c r="I31" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2155,32 +2340,34 @@
         <v>0</v>
       </c>
       <c r="K31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B32" t="n">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G32" t="n">
         <v>1</v>
       </c>
-      <c r="H32"/>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
       <c r="I32" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2188,21 +2375,21 @@
         <v>0</v>
       </c>
       <c r="K32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B33" t="n">
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E33" t="n">
         <v>2</v>
@@ -2211,7 +2398,9 @@
       <c r="G33" t="n">
         <v>2</v>
       </c>
-      <c r="H33"/>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
       <c r="I33" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2219,32 +2408,34 @@
         <v>0</v>
       </c>
       <c r="K33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B34" t="n">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E34" t="n">
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
       </c>
-      <c r="H34"/>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
       <c r="I34" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2252,32 +2443,34 @@
         <v>0</v>
       </c>
       <c r="K34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B35" t="n">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E35" t="n">
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G35" t="n">
         <v>1</v>
       </c>
-      <c r="H35"/>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
       <c r="I35" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2285,32 +2478,34 @@
         <v>0</v>
       </c>
       <c r="K35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B36" t="n">
         <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E36" t="n">
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="G36" t="n">
         <v>1</v>
       </c>
-      <c r="H36"/>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
       <c r="I36" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2318,32 +2513,34 @@
         <v>0</v>
       </c>
       <c r="K36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B37" t="n">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E37" t="n">
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G37" t="n">
         <v>1</v>
       </c>
-      <c r="H37"/>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
       <c r="I37" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2351,32 +2548,34 @@
         <v>0</v>
       </c>
       <c r="K37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B38" t="n">
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E38" t="n">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G38" t="n">
         <v>1</v>
       </c>
-      <c r="H38"/>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
       <c r="I38" s="1" t="n">
         <v>44659</v>
       </c>
@@ -2384,7 +2583,7 @@
         <v>0</v>
       </c>
       <c r="K38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>